<commit_message>
Merged in bugfix/update-status-adgroup-list (pull request #98)
Bugfix/update status adgroup list


Former-commit-id: f228a481d80e67492a6708e5b55885a5a4c4ac47
Former-commit-id: 713af0a547c9deb53f44de138eb01d932df804e9
</commit_message>
<xml_diff>
--- a/tests/resources/repo_yss_adgroup_report_cost.xlsx
+++ b/tests/resources/repo_yss_adgroup_report_cost.xlsx
@@ -191,57 +191,57 @@
       </c>
       <c r="I2" s="0" t="inlineStr">
         <is>
-          <t>20,969.22</t>
+          <t>79,976,616.95</t>
         </is>
       </c>
       <c r="J2" s="0" t="inlineStr">
         <is>
-          <t>20,751.39</t>
+          <t>79,145,809.76</t>
         </is>
       </c>
       <c r="K2" s="0" t="inlineStr">
         <is>
-          <t>21,073.96</t>
+          <t>80,376,068.20</t>
         </is>
       </c>
       <c r="L2" s="0" t="inlineStr">
         <is>
-          <t>20,940.83</t>
+          <t>79,868,341.35</t>
         </is>
       </c>
       <c r="M2" s="0" t="inlineStr">
         <is>
-          <t>20,617.43</t>
+          <t>78,634,868.31</t>
         </is>
       </c>
       <c r="N2" s="0" t="inlineStr">
         <is>
-          <t>21,041.98</t>
+          <t>80,254,117.59</t>
         </is>
       </c>
       <c r="O2" s="0" t="inlineStr">
         <is>
-          <t>20,816.23</t>
+          <t>79,393,109.68</t>
         </is>
       </c>
       <c r="P2" s="0" t="inlineStr">
         <is>
-          <t>20,664.71</t>
+          <t>78,815,218.77</t>
         </is>
       </c>
       <c r="Q2" s="0" t="inlineStr">
         <is>
-          <t>21,097.03</t>
+          <t>80,464,089.55</t>
         </is>
       </c>
       <c r="R2" s="0" t="inlineStr">
         <is>
-          <t>21,079.93</t>
+          <t>80,398,838.12</t>
         </is>
       </c>
       <c r="S2" s="0" t="inlineStr">
         <is>
-          <t>20,896.44</t>
+          <t>79,699,011.49</t>
         </is>
       </c>
     </row>
@@ -288,57 +288,57 @@
       </c>
       <c r="I3" s="0" t="inlineStr">
         <is>
-          <t>20,790.61</t>
+          <t>239,549,409.35</t>
         </is>
       </c>
       <c r="J3" s="0" t="inlineStr">
         <is>
-          <t>20,814.15</t>
+          <t>239,820,603.27</t>
         </is>
       </c>
       <c r="K3" s="0" t="inlineStr">
         <is>
-          <t>20,959.25</t>
+          <t>241,492,432.96</t>
         </is>
       </c>
       <c r="L3" s="0" t="inlineStr">
         <is>
-          <t>20,804.38</t>
+          <t>239,708,018.24</t>
         </is>
       </c>
       <c r="M3" s="0" t="inlineStr">
         <is>
-          <t>20,954.80</t>
+          <t>241,441,224.84</t>
         </is>
       </c>
       <c r="N3" s="0" t="inlineStr">
         <is>
-          <t>20,672.02</t>
+          <t>238,182,966.60</t>
         </is>
       </c>
       <c r="O3" s="0" t="inlineStr">
         <is>
-          <t>20,850.11</t>
+          <t>240,234,970.42</t>
         </is>
       </c>
       <c r="P3" s="0" t="inlineStr">
         <is>
-          <t>20,953.06</t>
+          <t>241,421,166.44</t>
         </is>
       </c>
       <c r="Q3" s="0" t="inlineStr">
         <is>
-          <t>20,780.85</t>
+          <t>239,436,983.89</t>
         </is>
       </c>
       <c r="R3" s="0" t="inlineStr">
         <is>
-          <t>20,781.84</t>
+          <t>239,448,383.43</t>
         </is>
       </c>
       <c r="S3" s="0" t="inlineStr">
         <is>
-          <t>20,702.66</t>
+          <t>238,536,048.93</t>
         </is>
       </c>
     </row>
@@ -385,57 +385,57 @@
       </c>
       <c r="I4" s="0" t="inlineStr">
         <is>
-          <t>21,003.65</t>
+          <t>242,004,004.60</t>
         </is>
       </c>
       <c r="J4" s="0" t="inlineStr">
         <is>
-          <t>20,820.91</t>
+          <t>239,898,473.56</t>
         </is>
       </c>
       <c r="K4" s="0" t="inlineStr">
         <is>
-          <t>20,743.69</t>
+          <t>239,008,833.36</t>
         </is>
       </c>
       <c r="L4" s="0" t="inlineStr">
         <is>
-          <t>20,638.36</t>
+          <t>237,795,169.88</t>
         </is>
       </c>
       <c r="M4" s="0" t="inlineStr">
         <is>
-          <t>20,734.78</t>
+          <t>238,906,165.35</t>
         </is>
       </c>
       <c r="N4" s="0" t="inlineStr">
         <is>
-          <t>20,890.21</t>
+          <t>240,697,047.84</t>
         </is>
       </c>
       <c r="O4" s="0" t="inlineStr">
         <is>
-          <t>20,776.02</t>
+          <t>239,381,295.54</t>
         </is>
       </c>
       <c r="P4" s="0" t="inlineStr">
         <is>
-          <t>20,698.93</t>
+          <t>238,493,110.07</t>
         </is>
       </c>
       <c r="Q4" s="0" t="inlineStr">
         <is>
-          <t>20,621.97</t>
+          <t>237,606,339.30</t>
         </is>
       </c>
       <c r="R4" s="0" t="inlineStr">
         <is>
-          <t>20,607.86</t>
+          <t>237,443,730.21</t>
         </is>
       </c>
       <c r="S4" s="0" t="inlineStr">
         <is>
-          <t>20,745.30</t>
+          <t>239,027,369.34</t>
         </is>
       </c>
     </row>
@@ -482,57 +482,57 @@
       </c>
       <c r="I5" s="0" t="inlineStr">
         <is>
-          <t>20,906.18</t>
+          <t>160,266,799.49</t>
         </is>
       </c>
       <c r="J5" s="0" t="inlineStr">
         <is>
-          <t>20,642.95</t>
+          <t>158,248,860.70</t>
         </is>
       </c>
       <c r="K5" s="0" t="inlineStr">
         <is>
-          <t>21,054.94</t>
+          <t>161,407,133.78</t>
         </is>
       </c>
       <c r="L5" s="0" t="inlineStr">
         <is>
-          <t>21,034.56</t>
+          <t>161,250,907.96</t>
         </is>
       </c>
       <c r="M5" s="0" t="inlineStr">
         <is>
-          <t>20,795.53</t>
+          <t>159,418,546.55</t>
         </is>
       </c>
       <c r="N5" s="0" t="inlineStr">
         <is>
-          <t>20,914.05</t>
+          <t>160,327,084.30</t>
         </is>
       </c>
       <c r="O5" s="0" t="inlineStr">
         <is>
-          <t>20,879.23</t>
+          <t>160,060,209.97</t>
         </is>
       </c>
       <c r="P5" s="0" t="inlineStr">
         <is>
-          <t>20,998.88</t>
+          <t>160,977,407.13</t>
         </is>
       </c>
       <c r="Q5" s="0" t="inlineStr">
         <is>
-          <t>21,123.96</t>
+          <t>161,936,277.26</t>
         </is>
       </c>
       <c r="R5" s="0" t="inlineStr">
         <is>
-          <t>20,878.67</t>
+          <t>160,055,872.03</t>
         </is>
       </c>
       <c r="S5" s="0" t="inlineStr">
         <is>
-          <t>20,885.00</t>
+          <t>160,104,398.94</t>
         </is>
       </c>
     </row>

</xml_diff>